<commit_message>
Add biomass to least cost dispatch electricity source subscript
</commit_message>
<xml_diff>
--- a/InputData/elec/ESUfRaLCD/Elec Sources Used for Rlbty and Lst Cst Dsptch.xlsx
+++ b/InputData/elec/ESUfRaLCD/Elec Sources Used for Rlbty and Lst Cst Dsptch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ESUfRaLCD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\ESUfRaLCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDBADE1-6DF0-4237-91E8-604F6BAE0255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB617001-EF01-48EB-97A1-E227BF801731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="2" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t xml:space="preserve">Sources: </t>
   </si>
@@ -176,13 +176,25 @@
   </si>
   <si>
     <t>municipal solid waste</t>
+  </si>
+  <si>
+    <t>We do not use nuclear for dispatch in the US because we have nuclear listed</t>
+  </si>
+  <si>
+    <t>as guaranteed dispatch in elec/BGDPbES.</t>
+  </si>
+  <si>
+    <t>biomass</t>
+  </si>
+  <si>
+    <t>biomass dispatch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +206,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,9 +238,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1D3264-BEAA-43D0-A5CC-06C5D3B72BE0}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +611,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -693,6 +713,16 @@
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1316,10 +1346,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,11 +1388,11 @@
         <v>44</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B21" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
+        <f t="shared" ref="B3:B22" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
         <v>natural gas steam turbine es</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C66" si="1">IF(A3="","",CONCATENATE(A3," dispatch"))</f>
+        <f t="shared" ref="C3:C67" si="1">IF(A3="","",CONCATENATE(A3," dispatch"))</f>
         <v>natural gas steam turbine dispatch</v>
       </c>
     </row>
@@ -1381,103 +1411,104 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>petroleum es</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="1"/>
-        <v>petroleum dispatch</v>
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>natural gas peaker es</v>
+        <v>petroleum es</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
-        <v>natural gas peaker dispatch</v>
+        <v>petroleum dispatch</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>lignite es</v>
+        <v>natural gas peaker es</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
-        <v>lignite dispatch</v>
+        <v>natural gas peaker dispatch</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>municipal solid waste es</v>
+        <v>lignite es</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
-        <v>municipal solid waste dispatch</v>
+        <v>lignite dispatch</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v>small modular reactor es</v>
+        <v>municipal solid waste es</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
-        <v>small modular reactor dispatch</v>
+        <v>municipal solid waste dispatch</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>hydrogen combustion turbine es</v>
+        <v>small modular reactor es</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
-        <v>hydrogen combustion turbine dispatch</v>
+        <v>small modular reactor dispatch</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>hydrogen combustion turbine es</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>hydrogen combustion turbine dispatch</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v>hydrogen combined cycle es</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C12" t="str">
         <f t="shared" si="1"/>
         <v>hydrogen combined cycle dispatch</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1571,6 +1602,10 @@
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -1842,13 +1877,13 @@
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" t="str">
-        <f t="shared" ref="C67:C80" si="2">IF(A67="","",CONCATENATE(A67," dispatch"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C68:C81" si="2">IF(A68="","",CONCATENATE(A68," dispatch"))</f>
         <v/>
       </c>
     </row>
@@ -1920,6 +1955,12 @@
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
Edit RAF for hydrogen power plants and enable CCS power plants for reliability pass
</commit_message>
<xml_diff>
--- a/InputData/elec/ESUfRaLCD/Elec Sources Used for Rlbty and Lst Cst Dsptch.xlsx
+++ b/InputData/elec/ESUfRaLCD/Elec Sources Used for Rlbty and Lst Cst Dsptch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ESUfRaLCD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\ESUfRaLCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233D45BA-BAED-45ED-ABE9-9BA92A98D952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1865FA8B-2E99-4F62-ADD7-E0855899DE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t xml:space="preserve">Sources: </t>
   </si>
@@ -194,6 +194,24 @@
   </si>
   <si>
     <t>hydro dispatch</t>
+  </si>
+  <si>
+    <t>hard coal w ccs es</t>
+  </si>
+  <si>
+    <t>natural gas combined cycle w ccs es</t>
+  </si>
+  <si>
+    <t>hard coal w ccs</t>
+  </si>
+  <si>
+    <t>natural gas combined cycle w ccs</t>
+  </si>
+  <si>
+    <t>biomass w ccs</t>
+  </si>
+  <si>
+    <t>lignite w ccs</t>
   </si>
 </sst>
 </file>
@@ -266,9 +284,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -306,7 +324,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -412,7 +430,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -554,7 +572,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1D3264-BEAA-43D0-A5CC-06C5D3B72BE0}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,10 +759,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,11 +800,11 @@
         <v>30</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B21" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
+        <f t="shared" ref="B3:B25" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
         <v>onshore wind es</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C66" si="1">IF(A3="","",CONCATENATE(A3," power plants"))</f>
+        <f t="shared" ref="C3:C70" si="1">IF(A3="","",CONCATENATE(A3," power plants"))</f>
         <v>onshore wind power plants</v>
       </c>
     </row>
@@ -844,68 +862,76 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>hydrogen combustion turbine es</v>
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
-        <v>hydrogen combustion turbine power plants</v>
+        <v>hard coal w ccs power plants</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>natural gas combined cycle w ccs power plants</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>biomass w ccs power plants</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>lignite w ccs power plants</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>hydrogen combustion turbine es</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>hydrogen combustion turbine power plants</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v>hydrogen combined cycle es</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C13" t="str">
         <f t="shared" si="1"/>
         <v>hydrogen combined cycle power plants</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -989,24 +1015,40 @@
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C25" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -1260,31 +1302,31 @@
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" t="str">
-        <f t="shared" ref="C67:C80" si="2">IF(A67="","",CONCATENATE(A67," power plants"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C71:C84" si="2">IF(A71="","",CONCATENATE(A71," power plants"))</f>
         <v/>
       </c>
     </row>
@@ -1338,6 +1380,30 @@
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C83" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
Remove peaker plants from sources used for least cost dispatch
</commit_message>
<xml_diff>
--- a/InputData/elec/ESUfRaLCD/Elec Sources Used for Rlbty and Lst Cst Dsptch.xlsx
+++ b/InputData/elec/ESUfRaLCD/Elec Sources Used for Rlbty and Lst Cst Dsptch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\ESUfRaLCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1865FA8B-2E99-4F62-ADD7-E0855899DE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471C0641-26B1-4907-BD24-F93E2DB8257A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t xml:space="preserve">Sources: </t>
   </si>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>hard coal</t>
-  </si>
-  <si>
-    <t>natural gas steam turbine</t>
   </si>
   <si>
     <t>lignite</t>
@@ -582,18 +579,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1D3264-BEAA-43D0-A5CC-06C5D3B72BE0}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A29" sqref="A29:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -601,7 +598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -609,144 +606,144 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -761,17 +758,17 @@
   </sheetPr>
   <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -782,7 +779,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -795,7 +792,7 @@
         <v>natural gas combined cycle power plants</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -808,7 +805,7 @@
         <v>onshore wind power plants</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -821,7 +818,7 @@
         <v>solar PV power plants</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -834,7 +831,7 @@
         <v>petroleum power plants</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -847,7 +844,7 @@
         <v>natural gas peaker power plants</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -860,33 +857,33 @@
         <v>small modular reactor power plants</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>hard coal w ccs power plants</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>55</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="C8" t="str">
-        <f t="shared" si="1"/>
-        <v>hard coal w ccs power plants</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>natural gas combined cycle w ccs power plants</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>56</v>
-      </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="1"/>
-        <v>natural gas combined cycle w ccs power plants</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -896,9 +893,9 @@
         <v>biomass w ccs power plants</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
@@ -908,7 +905,7 @@
         <v>lignite w ccs power plants</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -921,7 +918,7 @@
         <v>hydrogen combustion turbine power plants</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -934,7 +931,7 @@
         <v>hydrogen combined cycle power plants</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -944,7 +941,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -954,7 +951,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -964,7 +961,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -974,7 +971,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -984,7 +981,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -994,7 +991,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1004,7 +1001,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1014,7 +1011,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1024,7 +1021,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1034,7 +1031,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1044,7 +1041,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1054,355 +1051,355 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C38" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C44" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C46" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C47" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C48" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C49" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C50" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C51" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C53" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C54" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C55" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C56" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C57" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C58" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C60" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C62" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C63" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C64" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71" t="str">
         <f t="shared" ref="C71:C84" si="2">IF(A71="","",CONCATENATE(A71," power plants"))</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C72" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C74" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C75" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C77" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C78" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C79" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C80" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C81" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C82" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C83" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C84" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1418,19 +1415,19 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1442,7 +1439,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1455,146 +1452,137 @@
         <v>hard coal dispatch</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B20" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
+        <v>natural gas combined cycle es</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C65" si="1">IF(A3="","",CONCATENATE(A3," dispatch"))</f>
+        <v>natural gas combined cycle dispatch</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B23" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
-        <v>natural gas steam turbine es</v>
-      </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C68" si="1">IF(A3="","",CONCATENATE(A3," dispatch"))</f>
-        <v>natural gas steam turbine dispatch</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>natural gas combined cycle es</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" si="1"/>
-        <v>natural gas combined cycle dispatch</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>lignite es</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>lignite dispatch</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>petroleum es</v>
+        <v>municipal solid waste es</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
-        <v>petroleum dispatch</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>municipal solid waste dispatch</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>natural gas peaker es</v>
+        <v>small modular reactor es</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
-        <v>natural gas peaker dispatch</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>small modular reactor dispatch</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v>lignite es</v>
+        <v>hydrogen combustion turbine es</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
-        <v>lignite dispatch</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>hydrogen combustion turbine dispatch</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>municipal solid waste es</v>
+        <v>hydrogen combined cycle es</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
-        <v>municipal solid waste dispatch</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
+        <v>hydrogen combined cycle dispatch</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>small modular reactor es</v>
+        <v/>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
-        <v>small modular reactor dispatch</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v>hydrogen combustion turbine es</v>
+        <v/>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
-        <v>hydrogen combustion turbine dispatch</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>hydrogen combined cycle es</v>
+        <v/>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
-        <v>hydrogen combined cycle dispatch</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1604,7 +1592,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1614,7 +1602,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1624,7 +1612,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1634,7 +1622,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1644,7 +1632,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1654,7 +1642,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1664,386 +1652,356 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C21" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C22" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C25" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C38" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C44" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C46" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C47" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C48" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C49" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C50" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C51" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C53" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C54" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C55" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C56" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C57" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C58" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C60" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C62" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C63" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C64" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C66:C79" si="2">IF(A66="","",CONCATENATE(A66," dispatch"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69" t="str">
-        <f t="shared" ref="C69:C82" si="2">IF(A69="","",CONCATENATE(A69," dispatch"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C72" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C74" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C75" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C77" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C78" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C79" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C80" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C82" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
Revert "Remove peaker plants from sources used for least cost dispatch"
This reverts commit bf43cd03087894ff5a72d87fa12221caf067df84.
</commit_message>
<xml_diff>
--- a/InputData/elec/ESUfRaLCD/Elec Sources Used for Rlbty and Lst Cst Dsptch.xlsx
+++ b/InputData/elec/ESUfRaLCD/Elec Sources Used for Rlbty and Lst Cst Dsptch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\ESUfRaLCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471C0641-26B1-4907-BD24-F93E2DB8257A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1865FA8B-2E99-4F62-ADD7-E0855899DE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t xml:space="preserve">Sources: </t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>hard coal</t>
+  </si>
+  <si>
+    <t>natural gas steam turbine</t>
   </si>
   <si>
     <t>lignite</t>
@@ -579,18 +582,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1D3264-BEAA-43D0-A5CC-06C5D3B72BE0}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -598,7 +601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -606,144 +609,144 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -758,17 +761,17 @@
   </sheetPr>
   <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -779,7 +782,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -792,7 +795,7 @@
         <v>natural gas combined cycle power plants</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -805,7 +808,7 @@
         <v>onshore wind power plants</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -818,7 +821,7 @@
         <v>solar PV power plants</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -831,7 +834,7 @@
         <v>petroleum power plants</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -844,7 +847,7 @@
         <v>natural gas peaker power plants</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -857,33 +860,33 @@
         <v>small modular reactor power plants</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>hard coal w ccs power plants</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
         <v>54</v>
       </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="1"/>
-        <v>hard coal w ccs power plants</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>53</v>
-      </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
         <v>natural gas combined cycle w ccs power plants</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -893,9 +896,9 @@
         <v>biomass w ccs power plants</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
@@ -905,7 +908,7 @@
         <v>lignite w ccs power plants</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -918,7 +921,7 @@
         <v>hydrogen combustion turbine power plants</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -931,7 +934,7 @@
         <v>hydrogen combined cycle power plants</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -941,7 +944,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -951,7 +954,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -961,7 +964,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -971,7 +974,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -981,7 +984,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -991,7 +994,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1001,7 +1004,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1011,7 +1014,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1021,7 +1024,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1031,7 +1034,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1041,7 +1044,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1051,355 +1054,355 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" t="str">
         <f t="shared" ref="C71:C84" si="2">IF(A71="","",CONCATENATE(A71," power plants"))</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1415,19 +1418,19 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1439,7 +1442,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1452,137 +1455,146 @@
         <v>hard coal dispatch</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B23" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
+        <v>natural gas steam turbine es</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C68" si="1">IF(A3="","",CONCATENATE(A3," dispatch"))</f>
+        <v>natural gas steam turbine dispatch</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B20" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
         <v>natural gas combined cycle es</v>
       </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C65" si="1">IF(A3="","",CONCATENATE(A3," dispatch"))</f>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
         <v>natural gas combined cycle dispatch</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>50</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" t="str">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>petroleum es</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>petroleum dispatch</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>natural gas peaker es</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>natural gas peaker dispatch</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>lignite es</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C9" t="str">
         <f t="shared" si="1"/>
         <v>lignite dispatch</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" t="str">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>municipal solid waste es</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C10" t="str">
         <f t="shared" si="1"/>
         <v>municipal solid waste dispatch</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>small modular reactor es</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C11" t="str">
         <f t="shared" si="1"/>
         <v>small modular reactor dispatch</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v>hydrogen combustion turbine es</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C12" t="str">
         <f t="shared" si="1"/>
         <v>hydrogen combustion turbine dispatch</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v>hydrogen combined cycle es</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C13" t="str">
         <f t="shared" si="1"/>
         <v>hydrogen combined cycle dispatch</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1592,7 +1604,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1602,7 +1614,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1612,7 +1624,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1622,7 +1634,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1632,7 +1644,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1642,7 +1654,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1652,356 +1664,386 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C21" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" t="str">
-        <f t="shared" ref="C66:C79" si="2">IF(A66="","",CONCATENATE(A66," dispatch"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+        <f t="shared" ref="C69:C82" si="2">IF(A69="","",CONCATENATE(A69," dispatch"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
Add CCS plants to elec sources used for reliability subscript
</commit_message>
<xml_diff>
--- a/InputData/elec/ESUfRaLCD/Elec Sources Used for Rlbty and Lst Cst Dsptch.xlsx
+++ b/InputData/elec/ESUfRaLCD/Elec Sources Used for Rlbty and Lst Cst Dsptch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\ESUfRaLCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1865FA8B-2E99-4F62-ADD7-E0855899DE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D961C3-4FB2-4D97-827D-D4025E9BBF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t xml:space="preserve">Sources: </t>
   </si>
@@ -582,18 +582,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1D3264-BEAA-43D0-A5CC-06C5D3B72BE0}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A29" sqref="A29:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -601,7 +601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -609,142 +609,142 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -761,17 +761,17 @@
   </sheetPr>
   <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -782,7 +782,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -795,7 +795,7 @@
         <v>natural gas combined cycle power plants</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -808,7 +808,7 @@
         <v>onshore wind power plants</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -821,7 +821,7 @@
         <v>solar PV power plants</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -834,7 +834,7 @@
         <v>petroleum power plants</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -847,7 +847,7 @@
         <v>natural gas peaker power plants</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -860,7 +860,7 @@
         <v>small modular reactor power plants</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -872,7 +872,7 @@
         <v>hard coal w ccs power plants</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -884,7 +884,7 @@
         <v>natural gas combined cycle w ccs power plants</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -896,7 +896,7 @@
         <v>biomass w ccs power plants</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -908,7 +908,7 @@
         <v>lignite w ccs power plants</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -921,7 +921,7 @@
         <v>hydrogen combustion turbine power plants</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -934,7 +934,7 @@
         <v>hydrogen combined cycle power plants</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -944,7 +944,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -954,7 +954,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -964,7 +964,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -974,7 +974,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -984,7 +984,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -994,7 +994,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1004,7 +1004,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1014,7 +1014,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1024,7 +1024,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1034,7 +1034,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1044,7 +1044,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1054,355 +1054,355 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C38" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C44" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C46" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C47" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C48" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C49" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C50" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C51" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C53" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C54" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C55" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C56" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C57" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C58" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C60" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C62" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C63" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C64" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71" t="str">
         <f t="shared" ref="C71:C84" si="2">IF(A71="","",CONCATENATE(A71," power plants"))</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C72" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C74" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C75" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C77" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C78" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C79" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C80" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C81" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C82" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C83" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C84" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1418,19 +1418,19 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1442,7 +1442,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1455,20 +1455,20 @@
         <v>hard coal dispatch</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>44</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B23" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
+        <f t="shared" ref="B3:B27" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
         <v>natural gas steam turbine es</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C68" si="1">IF(A3="","",CONCATENATE(A3," dispatch"))</f>
+        <f t="shared" ref="C3:C72" si="1">IF(A3="","",CONCATENATE(A3," dispatch"))</f>
         <v>natural gas steam turbine dispatch</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>natural gas combined cycle dispatch</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>petroleum dispatch</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>natural gas peaker dispatch</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>lignite dispatch</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1555,86 +1555,94 @@
         <v>municipal solid waste dispatch</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>hard coal w ccs dispatch</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>natural gas combined cycle w ccs dispatch</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>biomass w ccs dispatch</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>lignite w ccs dispatch</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>small modular reactor es</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C15" t="str">
         <f t="shared" si="1"/>
         <v>small modular reactor dispatch</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v>hydrogen combustion turbine es</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C16" t="str">
         <f t="shared" si="1"/>
         <v>hydrogen combustion turbine dispatch</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v>hydrogen combined cycle es</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C17" t="str">
         <f t="shared" si="1"/>
         <v>hydrogen combined cycle dispatch</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1644,7 +1652,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1654,7 +1662,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1664,7 +1672,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1674,7 +1682,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1684,7 +1692,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1694,356 +1702,396 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C24" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C25" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C38" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C44" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C46" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C47" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C48" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C49" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C50" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C51" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C53" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C54" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C55" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C56" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C57" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C58" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C60" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C62" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C63" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C64" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69" t="str">
-        <f t="shared" ref="C69:C82" si="2">IF(A69="","",CONCATENATE(A69," dispatch"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C72" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C73:C86" si="2">IF(A73="","",CONCATENATE(A73," dispatch"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C74" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C75" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C77" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C78" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C79" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C80" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C81" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C82" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C83" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C84" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C85" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C86" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
remvove blank rows and column from subscript definition csv
</commit_message>
<xml_diff>
--- a/InputData/elec/ESUfRaLCD/Elec Sources Used for Rlbty and Lst Cst Dsptch.xlsx
+++ b/InputData/elec/ESUfRaLCD/Elec Sources Used for Rlbty and Lst Cst Dsptch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\ESUfRaLCD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/todd/eps/eps-us/InputData/elec/ESUfRaLCD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D961C3-4FB2-4D97-827D-D4025E9BBF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26578C50-7F18-C947-84CA-18CC1CD39ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -582,18 +582,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1D3264-BEAA-43D0-A5CC-06C5D3B72BE0}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -601,7 +601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -609,142 +609,142 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -765,13 +765,13 @@
       <selection activeCell="A8" sqref="A8:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -782,7 +782,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -795,7 +795,7 @@
         <v>natural gas combined cycle power plants</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -808,7 +808,7 @@
         <v>onshore wind power plants</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -821,7 +821,7 @@
         <v>solar PV power plants</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -834,7 +834,7 @@
         <v>petroleum power plants</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -847,7 +847,7 @@
         <v>natural gas peaker power plants</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -860,7 +860,7 @@
         <v>small modular reactor power plants</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -872,7 +872,7 @@
         <v>hard coal w ccs power plants</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -884,7 +884,7 @@
         <v>natural gas combined cycle w ccs power plants</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -896,7 +896,7 @@
         <v>biomass w ccs power plants</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -908,7 +908,7 @@
         <v>lignite w ccs power plants</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -921,7 +921,7 @@
         <v>hydrogen combustion turbine power plants</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -934,7 +934,7 @@
         <v>hydrogen combined cycle power plants</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -944,7 +944,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -954,7 +954,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -964,7 +964,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -974,7 +974,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -984,7 +984,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -994,7 +994,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1004,7 +1004,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1014,7 +1014,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1024,7 +1024,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1034,7 +1034,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1044,7 +1044,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1054,355 +1054,355 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C26" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C29" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C30" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C32" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C35" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C38" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C39" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C40" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C41" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C42" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C44" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C45" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C46" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C47" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C48" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C49" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C50" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C51" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C53" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C54" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C55" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C56" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C57" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C58" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C60" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C62" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C63" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C64" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C65" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C66" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C67" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C68" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C69" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C70" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C71" t="str">
         <f t="shared" ref="C71:C84" si="2">IF(A71="","",CONCATENATE(A71," power plants"))</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C72" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C73" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C74" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C75" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C76" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C77" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C78" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C79" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C80" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C81" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C82" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C83" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C84" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1418,19 +1418,19 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1440,9 +1440,8 @@
       <c r="C1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1455,20 +1454,20 @@
         <v>hard coal dispatch</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B27" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
+        <f t="shared" ref="B3:B17" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
         <v>natural gas steam turbine es</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C72" si="1">IF(A3="","",CONCATENATE(A3," dispatch"))</f>
+        <f t="shared" ref="C3:C17" si="1">IF(A3="","",CONCATENATE(A3," dispatch"))</f>
         <v>natural gas steam turbine dispatch</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1481,7 +1480,7 @@
         <v>natural gas combined cycle dispatch</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -1492,7 +1491,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1503,7 +1502,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1516,7 +1515,7 @@
         <v>petroleum dispatch</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1529,7 +1528,7 @@
         <v>natural gas peaker dispatch</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1542,7 +1541,7 @@
         <v>lignite dispatch</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1555,7 +1554,7 @@
         <v>municipal solid waste dispatch</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1567,7 +1566,7 @@
         <v>hard coal w ccs dispatch</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1579,7 +1578,7 @@
         <v>natural gas combined cycle w ccs dispatch</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -1591,7 +1590,7 @@
         <v>biomass w ccs dispatch</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>lignite w ccs dispatch</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1616,7 +1615,7 @@
         <v>small modular reactor dispatch</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1629,7 +1628,7 @@
         <v>hydrogen combustion turbine dispatch</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1640,460 +1639,6 @@
       <c r="C17" t="str">
         <f t="shared" si="1"/>
         <v>hydrogen combined cycle dispatch</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B23" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B24" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B25" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C27" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C29" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C30" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C31" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C32" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C34" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C35" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C38" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C39" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C40" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C41" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C42" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C43" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C45" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C46" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C47" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C48" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C49" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C50" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C51" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C52" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C53" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C54" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C55" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C56" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C57" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C58" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C59" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C61" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C62" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C63" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C64" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C65" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C66" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C68" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C69" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C70" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C71" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C72" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C73" t="str">
-        <f t="shared" ref="C73:C86" si="2">IF(A73="","",CONCATENATE(A73," dispatch"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C74" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C75" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C76" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C77" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C78" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C79" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C80" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C81" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C82" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C83" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C84" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C85" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C86" t="str">
-        <f t="shared" si="2"/>
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>